<commit_message>
nueva estructura base de datos
</commit_message>
<xml_diff>
--- a/Modo BBDD-GRUPO-5.xlsx
+++ b/Modo BBDD-GRUPO-5.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WEB-PROGRAMACION\001-ESTUDIANDO\FundacionGuacurari\InstSupPolitecnicoCba\proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WEB-PROGRAMACION\001-ESTUDIANDO\FundacionGuacurari\InstSupPolitecnicoCba\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14250" windowHeight="11955"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14250" windowHeight="11955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="76">
   <si>
     <t>ENTIDADES</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Provincia</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>Cuentas</t>
   </si>
   <si>
@@ -129,12 +126,6 @@
     <t>direccion</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>fecha_password</t>
-  </si>
-  <si>
     <t>id_login</t>
   </si>
   <si>
@@ -241,13 +232,34 @@
   </si>
   <si>
     <t>id_tipo_dni</t>
+  </si>
+  <si>
+    <t>Comisiones</t>
+  </si>
+  <si>
+    <t>valor_comision</t>
+  </si>
+  <si>
+    <t>Varchar</t>
+  </si>
+  <si>
+    <t>id_comision</t>
+  </si>
+  <si>
+    <t>passw</t>
+  </si>
+  <si>
+    <t>fecha_passw</t>
+  </si>
+  <si>
+    <t>mail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,8 +313,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +348,29 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -422,11 +464,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -477,10 +520,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -498,13 +537,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF00FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4730,8 +4790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:X57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4773,38 +4833,38 @@
   <sheetData>
     <row r="2" spans="2:24" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="2:24" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="47"/>
       <c r="J3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="18"/>
-      <c r="L3" s="19"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="47"/>
       <c r="N3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="36"/>
-      <c r="P3" s="37"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="47"/>
       <c r="R3" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="S3" s="36"/>
-      <c r="T3" s="37"/>
+        <v>6</v>
+      </c>
+      <c r="S3" s="57"/>
+      <c r="T3" s="47"/>
       <c r="V3" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="W3" s="36"/>
-      <c r="X3" s="37"/>
+        <v>5</v>
+      </c>
+      <c r="W3" s="57"/>
+      <c r="X3" s="47"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F4" s="20"/>
@@ -4814,98 +4874,98 @@
       <c r="K4" s="8"/>
       <c r="L4" s="21"/>
       <c r="N4" s="20"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="39"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="37"/>
       <c r="R4" s="20"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="39"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="37"/>
       <c r="V4" s="20"/>
-      <c r="W4" s="38"/>
-      <c r="X4" s="39"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="37"/>
     </row>
     <row r="5" spans="2:24" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H5" s="23"/>
       <c r="J5" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L5" s="23"/>
       <c r="N5" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O5" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="P5" s="23"/>
       <c r="R5" s="22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="T5" s="23"/>
       <c r="V5" s="22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="W5" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="X5" s="23"/>
     </row>
     <row r="6" spans="2:24" ht="18" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="F6" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H6" s="24">
         <v>50</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L6" s="24">
         <v>50</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="P6" s="24">
         <v>50</v>
       </c>
-      <c r="R6" s="20" t="s">
-        <v>4</v>
+      <c r="R6" s="50" t="s">
+        <v>75</v>
       </c>
       <c r="S6" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="T6" s="24">
         <v>50</v>
       </c>
       <c r="V6" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="W6" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="X6" s="24">
         <v>50</v>
@@ -4916,55 +4976,55 @@
         <v>1</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H7" s="24">
         <v>50</v>
       </c>
       <c r="J7" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K7" s="32" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L7" s="33">
         <v>50</v>
       </c>
       <c r="N7" s="31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O7" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="P7" s="40"/>
+        <v>55</v>
+      </c>
+      <c r="P7" s="38"/>
       <c r="R7" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="S7" s="41" t="s">
-        <v>58</v>
+        <v>64</v>
+      </c>
+      <c r="S7" s="39" t="s">
+        <v>55</v>
       </c>
       <c r="T7" s="33"/>
       <c r="V7" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="W7" s="41" t="s">
-        <v>58</v>
+        <v>64</v>
+      </c>
+      <c r="W7" s="39" t="s">
+        <v>55</v>
       </c>
       <c r="X7" s="33"/>
     </row>
     <row r="8" spans="2:24" ht="18" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="D8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H8" s="24"/>
       <c r="K8" s="13"/>
@@ -4975,13 +5035,13 @@
         <v>3</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H9" s="26">
         <v>50</v>
@@ -4991,351 +5051,353 @@
     <row r="10" spans="2:24" ht="18" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="D10" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H10" s="27">
         <v>50</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" s="34"/>
-      <c r="L10" s="35"/>
+        <v>29</v>
+      </c>
+      <c r="K10" s="56"/>
+      <c r="L10" s="48"/>
       <c r="N10" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="O10" s="36"/>
-      <c r="P10" s="37"/>
+        <v>47</v>
+      </c>
+      <c r="O10" s="58"/>
+      <c r="P10" s="47"/>
       <c r="R10" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="S10" s="36"/>
-      <c r="T10" s="37"/>
+        <v>51</v>
+      </c>
+      <c r="S10" s="57"/>
+      <c r="T10" s="47"/>
     </row>
     <row r="11" spans="2:24" ht="18" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H11" s="27"/>
       <c r="J11" s="20"/>
       <c r="K11" s="8"/>
       <c r="L11" s="27"/>
       <c r="N11" s="20"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="39"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="37"/>
       <c r="R11" s="20"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="39"/>
+      <c r="S11" s="36"/>
+      <c r="T11" s="37"/>
     </row>
     <row r="12" spans="2:24" ht="18" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="F12" s="20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H12" s="27">
         <v>50</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L12" s="23"/>
       <c r="N12" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O12" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="P12" s="23"/>
       <c r="R12" s="22" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="S12" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="T12" s="23"/>
+      <c r="V12" s="11"/>
     </row>
     <row r="13" spans="2:24" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H13" s="26"/>
       <c r="J13" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="K13" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="L13" s="43">
+        <v>8</v>
+      </c>
+      <c r="K13" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="L13" s="41">
         <v>50</v>
       </c>
       <c r="N13" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="O13" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="P13" s="43">
+        <v>23</v>
+      </c>
+      <c r="O13" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="P13" s="41">
         <v>50</v>
       </c>
       <c r="R13" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="S13" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="T13" s="43">
+        <v>23</v>
+      </c>
+      <c r="S13" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="T13" s="41">
         <v>50</v>
       </c>
     </row>
     <row r="14" spans="2:24" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="F14" s="25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H14" s="26"/>
       <c r="L14" s="12"/>
     </row>
     <row r="15" spans="2:24" ht="18" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H15" s="26"/>
       <c r="J15" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="K15" s="36"/>
-      <c r="L15" s="37"/>
+        <v>4</v>
+      </c>
+      <c r="K15" s="34"/>
+      <c r="L15" s="35"/>
       <c r="N15" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="O15" s="36"/>
-      <c r="P15" s="37"/>
+        <v>7</v>
+      </c>
+      <c r="O15" s="58"/>
+      <c r="P15" s="47"/>
       <c r="R15" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="S15" s="36"/>
-      <c r="T15" s="37"/>
+        <v>50</v>
+      </c>
+      <c r="S15" s="34"/>
+      <c r="T15" s="35"/>
     </row>
     <row r="16" spans="2:24" ht="18" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="F16" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H16" s="26"/>
       <c r="J16" s="20"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="39"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="37"/>
       <c r="N16" s="20"/>
-      <c r="O16" s="38"/>
-      <c r="P16" s="39"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="37"/>
       <c r="R16" s="20"/>
-      <c r="S16" s="38"/>
-      <c r="T16" s="39"/>
+      <c r="S16" s="36"/>
+      <c r="T16" s="37"/>
     </row>
     <row r="17" spans="2:20" ht="18" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H17" s="26"/>
       <c r="J17" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="L17" s="39"/>
+        <v>55</v>
+      </c>
+      <c r="L17" s="37"/>
       <c r="N17" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O17" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="P17" s="39"/>
+        <v>55</v>
+      </c>
+      <c r="P17" s="37"/>
       <c r="R17" s="22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="S17" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="T17" s="39"/>
+        <v>55</v>
+      </c>
+      <c r="T17" s="37"/>
     </row>
     <row r="18" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F18" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H18" s="26"/>
-      <c r="J18" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="K18" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="L18" s="39"/>
+      <c r="J18" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="L18" s="54">
+        <v>22</v>
+      </c>
       <c r="N18" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="O18" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="O18" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="P18" s="41">
+        <v>50</v>
+      </c>
+      <c r="R18" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="S18" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="P18" s="43">
-        <v>50</v>
-      </c>
-      <c r="R18" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="S18" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="T18" s="39"/>
+      <c r="T18" s="37"/>
     </row>
     <row r="19" spans="2:20" ht="18" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H19" s="26"/>
       <c r="J19" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="L19" s="39"/>
+        <v>55</v>
+      </c>
+      <c r="L19" s="37"/>
       <c r="R19" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S19" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="T19" s="24">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F20" s="20" t="s">
-        <v>34</v>
+      <c r="F20" s="50" t="s">
+        <v>73</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H20" s="27">
         <v>50</v>
       </c>
       <c r="J20" s="31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K20" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="L20" s="40"/>
+        <v>55</v>
+      </c>
+      <c r="L20" s="38"/>
       <c r="R20" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S20" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="T20" s="39"/>
+        <v>55</v>
+      </c>
+      <c r="T20" s="37"/>
     </row>
     <row r="21" spans="2:20" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>35</v>
+        <v>51</v>
+      </c>
+      <c r="F21" s="59" t="s">
+        <v>74</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H21" s="30"/>
       <c r="J21"/>
       <c r="K21"/>
       <c r="L21"/>
       <c r="R21" s="31" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="S21" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="T21" s="40"/>
+        <v>55</v>
+      </c>
+      <c r="T21" s="38"/>
     </row>
     <row r="22" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="11"/>
       <c r="R22"/>
     </row>
     <row r="23" spans="2:20" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="K23" s="18"/>
-      <c r="L23" s="19"/>
+        <v>39</v>
+      </c>
+      <c r="K23" s="57"/>
+      <c r="L23" s="49"/>
       <c r="N23" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="O23" s="36"/>
-      <c r="P23" s="37"/>
+        <v>36</v>
+      </c>
+      <c r="O23" s="34"/>
+      <c r="P23" s="35"/>
       <c r="R23" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="S23" s="36"/>
-      <c r="T23" s="37"/>
+        <v>53</v>
+      </c>
+      <c r="S23" s="34"/>
+      <c r="T23" s="35"/>
     </row>
     <row r="24" spans="2:20" ht="18" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="F24" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G24" s="18"/>
       <c r="H24" s="19"/>
@@ -5343,254 +5405,314 @@
       <c r="K24" s="8"/>
       <c r="L24" s="21"/>
       <c r="N24" s="20"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="39"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="37"/>
       <c r="R24" s="20"/>
-      <c r="S24" s="38"/>
-      <c r="T24" s="39"/>
+      <c r="S24" s="36"/>
+      <c r="T24" s="37"/>
     </row>
     <row r="25" spans="2:20" ht="18" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" s="44"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="39"/>
+        <v>4</v>
+      </c>
+      <c r="F25" s="42"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="37"/>
       <c r="J25" s="22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="L25" s="45"/>
+        <v>55</v>
+      </c>
+      <c r="L25" s="43"/>
       <c r="N25" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="O25" s="38"/>
-      <c r="P25" s="39"/>
+        <v>26</v>
+      </c>
+      <c r="O25" s="36"/>
+      <c r="P25" s="37"/>
       <c r="R25" s="22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="S25" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="T25" s="39"/>
+        <v>55</v>
+      </c>
+      <c r="T25" s="37"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="F26" s="22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="H26" s="45"/>
+        <v>55</v>
+      </c>
+      <c r="H26" s="43"/>
       <c r="J26" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L26" s="27">
         <v>50</v>
       </c>
       <c r="N26" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="O26" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="P26" s="37"/>
+      <c r="R26" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="S26" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="T26" s="37"/>
+    </row>
+    <row r="27" spans="2:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" s="37"/>
+      <c r="J27" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="K27" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="P26" s="39"/>
-      <c r="R26" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="S26" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="T26" s="39"/>
-    </row>
-    <row r="27" spans="2:20" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H27" s="39"/>
-      <c r="J27" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="K27" s="29"/>
-      <c r="L27" s="46"/>
+      <c r="L27" s="52"/>
       <c r="N27" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="P27" s="39"/>
+        <v>56</v>
+      </c>
+      <c r="P27" s="37"/>
       <c r="R27" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S27" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="T27" s="39"/>
+        <v>55</v>
+      </c>
+      <c r="T27" s="37"/>
     </row>
     <row r="28" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F28" s="20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H28" s="21"/>
+      <c r="J28" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="K28" s="29"/>
+      <c r="L28" s="44"/>
       <c r="N28" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="O28" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="P28" s="39"/>
+        <v>20</v>
+      </c>
+      <c r="O28" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="P28" s="37"/>
       <c r="R28" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="S28" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="T28" s="39"/>
+        <v>58</v>
+      </c>
+      <c r="T28" s="37"/>
     </row>
     <row r="29" spans="2:20" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G29" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="H29" s="46"/>
-      <c r="J29" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="K29" s="18"/>
-      <c r="L29" s="19"/>
+        <v>57</v>
+      </c>
+      <c r="H29" s="44"/>
       <c r="N29" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="O29" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="P29" s="39"/>
+        <v>55</v>
+      </c>
+      <c r="P29" s="37"/>
       <c r="R29" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="S29" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="S29" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="T29" s="37"/>
+    </row>
+    <row r="30" spans="2:20" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="57"/>
+      <c r="L30" s="49"/>
+      <c r="N30" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="O30" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="P30" s="37"/>
+      <c r="R30" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="S30" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="T29" s="39"/>
-    </row>
-    <row r="30" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J30" s="20"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="21"/>
-      <c r="N30" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="O30" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="P30" s="39"/>
-      <c r="R30" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="S30" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="T30" s="40"/>
+      <c r="T30" s="38"/>
     </row>
     <row r="31" spans="2:20" ht="18" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="55"/>
+      <c r="F31" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="18"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="21"/>
+      <c r="N31" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="O31" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="P31" s="37"/>
+      <c r="R31" s="8"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="E32" s="55"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="J31" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="K31" s="15" t="s">
+      <c r="K32" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="L32" s="43"/>
+      <c r="N32" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="O32" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="L31" s="45"/>
-      <c r="N31" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="O31" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="P31" s="39"/>
-      <c r="R31" s="8"/>
-    </row>
-    <row r="32" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J32" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="K32" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="L32" s="30">
+      <c r="P32" s="37"/>
+      <c r="R32" s="8"/>
+    </row>
+    <row r="33" spans="2:22" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="55"/>
+      <c r="F33" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H33" s="43"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="K33" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="L33" s="30">
         <v>50</v>
       </c>
-      <c r="N32" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="O32" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="P32" s="39"/>
-      <c r="R32" s="8"/>
-    </row>
-    <row r="33" spans="2:22" ht="18" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
+      <c r="N33" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="O33" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="P33" s="37"/>
+      <c r="R33" s="8"/>
+      <c r="U33" s="11"/>
+    </row>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="E34" s="55"/>
+      <c r="F34" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H34" s="37"/>
+      <c r="I34" s="55"/>
+      <c r="N34" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="N33" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="O33" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="P33" s="39"/>
-      <c r="R33" s="8"/>
-    </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="N34" s="25" t="s">
-        <v>45</v>
-      </c>
       <c r="O34" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="P34" s="39"/>
+        <v>55</v>
+      </c>
+      <c r="P34" s="37"/>
     </row>
     <row r="35" spans="2:22" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F35" s="11"/>
+        <v>36</v>
+      </c>
+      <c r="E35" s="55"/>
+      <c r="F35" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="H35" s="44"/>
+      <c r="I35" s="55"/>
       <c r="N35" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="O35" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="P35" s="40"/>
+        <v>38</v>
+      </c>
+      <c r="O35" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="P35" s="38"/>
       <c r="R35" s="9"/>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="11"/>
     </row>
     <row r="37" spans="2:22" ht="18" x14ac:dyDescent="0.25">
       <c r="B37" s="10" t="s">
-        <v>56</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="J37" s="11"/>
     </row>
     <row r="41" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B41"/>
@@ -5784,7 +5906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="P4:S24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
@@ -5847,7 +5969,7 @@
       <c r="S11"/>
     </row>
     <row r="12" spans="16:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="P12" s="48"/>
+      <c r="P12" s="46"/>
       <c r="Q12"/>
       <c r="R12"/>
       <c r="S12"/>

</xml_diff>

<commit_message>
cambios en bases de datos
</commit_message>
<xml_diff>
--- a/Modo BBDD-GRUPO-5.xlsx
+++ b/Modo BBDD-GRUPO-5.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14250" windowHeight="11955" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14250" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="81">
   <si>
     <t>ENTIDADES</t>
   </si>
@@ -72,9 +72,6 @@
     <t>fecha</t>
   </si>
   <si>
-    <t>estado (alta/baja/suspension)</t>
-  </si>
-  <si>
     <t>Cuentas_Historia_Estado</t>
   </si>
   <si>
@@ -138,24 +135,12 @@
     <t>Transacciones_Cuenta</t>
   </si>
   <si>
-    <t>monto1</t>
-  </si>
-  <si>
-    <t>monto2</t>
-  </si>
-  <si>
     <t>Tipo_Transaccion</t>
   </si>
   <si>
     <t>id_tipo_transaccion</t>
   </si>
   <si>
-    <t>id_moneda1</t>
-  </si>
-  <si>
-    <t>id_moneda2</t>
-  </si>
-  <si>
     <t>id_cuenta_destino</t>
   </si>
   <si>
@@ -246,20 +231,50 @@
     <t>id_comision</t>
   </si>
   <si>
-    <t>passw</t>
-  </si>
-  <si>
-    <t>fecha_passw</t>
-  </si>
-  <si>
     <t>mail</t>
+  </si>
+  <si>
+    <t>monto_comision</t>
+  </si>
+  <si>
+    <t>id_moneda_origen</t>
+  </si>
+  <si>
+    <t>monto_origen</t>
+  </si>
+  <si>
+    <t>id_moneda_destino</t>
+  </si>
+  <si>
+    <t>monto_destino</t>
+  </si>
+  <si>
+    <t>Tarjetas</t>
+  </si>
+  <si>
+    <t>id_tarjeta</t>
+  </si>
+  <si>
+    <t>numero_tarjeta</t>
+  </si>
+  <si>
+    <t>fecha_vencimiento</t>
+  </si>
+  <si>
+    <t>porcentaje_comision</t>
+  </si>
+  <si>
+    <t>clave</t>
+  </si>
+  <si>
+    <t>fecha_clave</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +331,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -469,7 +492,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -537,6 +560,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -552,6 +576,10 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -4481,19 +4509,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>150974</xdr:rowOff>
+      <xdr:rowOff>103770</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="79" name="Imagen 78"/>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4512,8 +4540,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="762000" y="85725"/>
-          <a:ext cx="10058400" cy="7323299"/>
+          <a:off x="1476375" y="180975"/>
+          <a:ext cx="10058400" cy="7180845"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4790,8 +4818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:X57"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4833,38 +4861,38 @@
   <sheetData>
     <row r="2" spans="2:24" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="2:24" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="57"/>
-      <c r="H3" s="47"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="48"/>
       <c r="J3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="57"/>
-      <c r="L3" s="47"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="48"/>
       <c r="N3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="57"/>
-      <c r="P3" s="47"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="48"/>
       <c r="R3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="S3" s="57"/>
-      <c r="T3" s="47"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="48"/>
       <c r="V3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="W3" s="57"/>
-      <c r="X3" s="47"/>
+      <c r="W3" s="58"/>
+      <c r="X3" s="48"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F4" s="20"/>
@@ -4888,38 +4916,38 @@
         <v>0</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H5" s="23"/>
       <c r="J5" s="22" t="s">
         <v>11</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="L5" s="23"/>
       <c r="N5" s="22" t="s">
         <v>10</v>
       </c>
       <c r="O5" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="P5" s="23"/>
       <c r="R5" s="22" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="T5" s="23"/>
       <c r="V5" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="W5" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="X5" s="23"/>
     </row>
@@ -4929,7 +4957,7 @@
         <v>8</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H6" s="24">
         <v>50</v>
@@ -4938,7 +4966,7 @@
         <v>8</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="L6" s="24">
         <v>50</v>
@@ -4947,16 +4975,16 @@
         <v>8</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="P6" s="24">
         <v>50</v>
       </c>
-      <c r="R6" s="50" t="s">
-        <v>75</v>
+      <c r="R6" s="51" t="s">
+        <v>68</v>
       </c>
       <c r="S6" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="T6" s="24">
         <v>50</v>
@@ -4965,7 +4993,7 @@
         <v>12</v>
       </c>
       <c r="W6" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="X6" s="24">
         <v>50</v>
@@ -4979,16 +5007,16 @@
         <v>9</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H7" s="24">
         <v>50</v>
       </c>
       <c r="J7" s="31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K7" s="32" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="L7" s="33">
         <v>50</v>
@@ -4997,34 +5025,34 @@
         <v>11</v>
       </c>
       <c r="O7" s="32" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="P7" s="38"/>
       <c r="R7" s="31" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="S7" s="39" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="T7" s="33"/>
       <c r="V7" s="31" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="W7" s="39" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="X7" s="33"/>
     </row>
     <row r="8" spans="2:24" ht="18" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="D8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H8" s="24"/>
       <c r="K8" s="13"/>
@@ -5035,13 +5063,13 @@
         <v>3</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H9" s="26">
         <v>50</v>
@@ -5051,42 +5079,42 @@
     <row r="10" spans="2:24" ht="18" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="D10" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H10" s="27">
         <v>50</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="K10" s="56"/>
-      <c r="L10" s="48"/>
+        <v>28</v>
+      </c>
+      <c r="K10" s="57"/>
+      <c r="L10" s="49"/>
       <c r="N10" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="O10" s="58"/>
-      <c r="P10" s="47"/>
+        <v>42</v>
+      </c>
+      <c r="O10" s="59"/>
+      <c r="P10" s="48"/>
       <c r="R10" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="S10" s="57"/>
-      <c r="T10" s="47"/>
+        <v>46</v>
+      </c>
+      <c r="S10" s="58"/>
+      <c r="T10" s="48"/>
     </row>
     <row r="11" spans="2:24" ht="18" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H11" s="27"/>
       <c r="J11" s="20"/>
@@ -5102,33 +5130,33 @@
     <row r="12" spans="2:24" ht="18" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="F12" s="20" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H12" s="27">
         <v>50</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="L12" s="23"/>
       <c r="N12" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O12" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="P12" s="23"/>
       <c r="R12" s="22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="S12" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="T12" s="23"/>
       <c r="V12" s="11"/>
@@ -5138,35 +5166,35 @@
         <v>6</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H13" s="26"/>
       <c r="J13" s="28" t="s">
         <v>8</v>
       </c>
       <c r="K13" s="40" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="L13" s="41">
         <v>50</v>
       </c>
       <c r="N13" s="28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O13" s="40" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="P13" s="41">
         <v>50</v>
       </c>
       <c r="R13" s="28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S13" s="40" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="T13" s="41">
         <v>50</v>
@@ -5175,10 +5203,10 @@
     <row r="14" spans="2:24" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="F14" s="25" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H14" s="26"/>
       <c r="L14" s="12"/>
@@ -5188,10 +5216,10 @@
         <v>5</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H15" s="26"/>
       <c r="J15" s="17" t="s">
@@ -5202,10 +5230,10 @@
       <c r="N15" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="O15" s="58"/>
-      <c r="P15" s="47"/>
+      <c r="O15" s="59"/>
+      <c r="P15" s="48"/>
       <c r="R15" s="17" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="S15" s="34"/>
       <c r="T15" s="35"/>
@@ -5216,7 +5244,7 @@
         <v>11</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H16" s="26"/>
       <c r="J16" s="20"/>
@@ -5229,175 +5257,176 @@
       <c r="S16" s="36"/>
       <c r="T16" s="37"/>
     </row>
-    <row r="17" spans="2:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:22" ht="18" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F17" s="25" t="s">
         <v>10</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H17" s="26"/>
       <c r="J17" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="L17" s="37"/>
       <c r="N17" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O17" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="P17" s="37"/>
       <c r="R17" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S17" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="T17" s="37"/>
     </row>
-    <row r="18" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F18" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H18" s="26"/>
-      <c r="J18" s="50" t="s">
+      <c r="J18" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="L18" s="54">
+      <c r="K18" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="L18" s="55">
         <v>22</v>
       </c>
       <c r="N18" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="O18" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="P18" s="41">
+        <v>50</v>
+      </c>
+      <c r="R18" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="S18" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="T18" s="37"/>
+    </row>
+    <row r="19" spans="2:22" ht="18" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="O18" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="P18" s="41">
-        <v>50</v>
-      </c>
-      <c r="R18" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="S18" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="T18" s="37"/>
-    </row>
-    <row r="19" spans="2:20" ht="18" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>28</v>
-      </c>
       <c r="G19" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H19" s="26"/>
       <c r="J19" s="25" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="L19" s="37"/>
-      <c r="R19" s="20" t="s">
-        <v>15</v>
+      <c r="R19" s="51" t="s">
+        <v>29</v>
       </c>
       <c r="S19" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="T19" s="24">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F20" s="50" t="s">
-        <v>73</v>
+    <row r="20" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="51" t="s">
+        <v>79</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H20" s="27">
         <v>50</v>
       </c>
       <c r="J20" s="31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K20" s="32" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="L20" s="38"/>
       <c r="R20" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S20" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="T20" s="37"/>
     </row>
-    <row r="21" spans="2:20" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:22" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" s="29" t="s">
         <v>51</v>
-      </c>
-      <c r="F21" s="59" t="s">
-        <v>74</v>
-      </c>
-      <c r="G21" s="29" t="s">
-        <v>56</v>
       </c>
       <c r="H21" s="30"/>
       <c r="J21"/>
       <c r="K21"/>
       <c r="L21"/>
       <c r="R21" s="31" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="S21" s="32" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="T21" s="38"/>
     </row>
-    <row r="22" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="R22"/>
     </row>
-    <row r="23" spans="2:20" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:22" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K23" s="58"/>
+      <c r="L23" s="50"/>
+      <c r="N23" s="17" t="s">
         <v>35</v>
-      </c>
-      <c r="J23" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="K23" s="57"/>
-      <c r="L23" s="49"/>
-      <c r="N23" s="17" t="s">
-        <v>36</v>
       </c>
       <c r="O23" s="34"/>
       <c r="P23" s="35"/>
       <c r="R23" s="17" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="S23" s="34"/>
       <c r="T23" s="35"/>
-    </row>
-    <row r="24" spans="2:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="V23" s="11"/>
+    </row>
+    <row r="24" spans="2:22" ht="18" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="F24" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G24" s="18"/>
       <c r="H24" s="19"/>
@@ -5411,7 +5440,7 @@
       <c r="S24" s="36"/>
       <c r="T24" s="37"/>
     </row>
-    <row r="25" spans="2:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:22" ht="18" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>4</v>
       </c>
@@ -5419,313 +5448,424 @@
       <c r="G25" s="36"/>
       <c r="H25" s="37"/>
       <c r="J25" s="22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="L25" s="43"/>
       <c r="N25" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O25" s="36"/>
       <c r="P25" s="37"/>
       <c r="R25" s="22" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="S25" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="T25" s="37"/>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
       <c r="F26" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H26" s="43"/>
       <c r="J26" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="L26" s="27">
         <v>50</v>
       </c>
       <c r="N26" s="25" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="O26" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="P26" s="37"/>
       <c r="R26" s="25" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="S26" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="T26" s="37"/>
     </row>
-    <row r="27" spans="2:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:22" ht="18" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H27" s="37"/>
-      <c r="J27" s="50" t="s">
-        <v>70</v>
-      </c>
-      <c r="K27" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="L27" s="52"/>
+      <c r="J27" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="K27" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="L27" s="53"/>
       <c r="N27" s="20" t="s">
         <v>14</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="P27" s="37"/>
       <c r="R27" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S27" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="T27" s="37"/>
     </row>
-    <row r="28" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F28" s="20" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H28" s="21"/>
       <c r="J28" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K28" s="29"/>
       <c r="L28" s="44"/>
       <c r="N28" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O28" s="36" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="P28" s="37"/>
       <c r="R28" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="S28" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="T28" s="37"/>
+    </row>
+    <row r="29" spans="2:22" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G29" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="S28" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="T28" s="37"/>
-    </row>
-    <row r="29" spans="2:20" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="G29" s="29" t="s">
-        <v>57</v>
-      </c>
       <c r="H29" s="44"/>
+      <c r="M29" s="56"/>
       <c r="N29" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="O29" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="P29" s="37"/>
+      <c r="Q29" s="56"/>
       <c r="R29" s="20" t="s">
         <v>14</v>
       </c>
       <c r="S29" s="36" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="T29" s="37"/>
     </row>
-    <row r="30" spans="2:20" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
+    <row r="30" spans="2:22" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
       <c r="J30" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="K30" s="57"/>
-      <c r="L30" s="49"/>
+        <v>20</v>
+      </c>
+      <c r="K30" s="58"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="56"/>
       <c r="N30" s="25" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O30" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="P30" s="37"/>
+      <c r="Q30" s="56"/>
       <c r="R30" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="S30" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="T30" s="38"/>
+    </row>
+    <row r="31" spans="2:22" ht="18" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="S30" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="T30" s="38"/>
-    </row>
-    <row r="31" spans="2:20" ht="18" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E31" s="55"/>
+      <c r="E31" s="56"/>
       <c r="F31" s="17" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G31" s="18"/>
       <c r="H31" s="19"/>
-      <c r="I31" s="55"/>
+      <c r="I31" s="56"/>
       <c r="J31" s="20"/>
       <c r="K31" s="8"/>
       <c r="L31" s="21"/>
+      <c r="M31" s="56"/>
       <c r="N31" s="25" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="O31" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="P31" s="37"/>
+      <c r="Q31" s="56"/>
       <c r="R31" s="8"/>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="E32" s="55"/>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="E32" s="56"/>
       <c r="F32" s="42"/>
       <c r="G32" s="36"/>
       <c r="H32" s="37"/>
-      <c r="I32" s="55"/>
+      <c r="I32" s="56"/>
       <c r="J32" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K32" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="L32" s="43"/>
+      <c r="M32" s="56"/>
       <c r="N32" s="20" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="P32" s="37"/>
+      <c r="Q32" s="56"/>
       <c r="R32" s="8"/>
     </row>
     <row r="33" spans="2:22" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="55"/>
+        <v>36</v>
+      </c>
+      <c r="E33" s="56"/>
       <c r="F33" s="22" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H33" s="43"/>
-      <c r="I33" s="55"/>
+      <c r="I33" s="56"/>
       <c r="J33" s="28" t="s">
         <v>8</v>
       </c>
       <c r="K33" s="29" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="L33" s="30">
         <v>50</v>
       </c>
+      <c r="M33" s="56"/>
       <c r="N33" s="25" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="O33" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="P33" s="37"/>
-      <c r="R33" s="8"/>
+      <c r="Q33" s="56"/>
+      <c r="R33" s="64"/>
       <c r="U33" s="11"/>
     </row>
     <row r="34" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="E34" s="55"/>
+      <c r="E34" s="56"/>
       <c r="F34" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H34" s="37"/>
-      <c r="I34" s="55"/>
+      <c r="I34" s="56"/>
+      <c r="M34" s="56"/>
       <c r="N34" s="25" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="O34" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="P34" s="37"/>
-    </row>
-    <row r="35" spans="2:22" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q34" s="56"/>
+      <c r="R34" s="11"/>
+    </row>
+    <row r="35" spans="2:22" ht="18" x14ac:dyDescent="0.25">
       <c r="B35" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="55"/>
-      <c r="F35" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="H35" s="44"/>
-      <c r="I35" s="55"/>
-      <c r="N35" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="O35" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="P35" s="38"/>
+        <v>35</v>
+      </c>
+      <c r="E35" s="56"/>
+      <c r="F35" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H35" s="21"/>
+      <c r="I35" s="56"/>
+      <c r="M35" s="56"/>
+      <c r="N35" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="O35" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="P35" s="37"/>
+      <c r="Q35" s="56"/>
       <c r="R35" s="9"/>
     </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="55"/>
+    <row r="36" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E36" s="56"/>
+      <c r="F36" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H36" s="21"/>
+      <c r="I36" s="56"/>
       <c r="J36" s="11"/>
+      <c r="M36" s="56"/>
+      <c r="N36" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O36" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="P36" s="38"/>
+      <c r="Q36" s="56"/>
     </row>
     <row r="37" spans="2:22" ht="18" x14ac:dyDescent="0.25">
       <c r="B37" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" s="56"/>
+      <c r="F37" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G37" s="8" t="s">
         <v>53</v>
       </c>
+      <c r="H37" s="21"/>
+      <c r="I37" s="56"/>
       <c r="J37" s="11"/>
-    </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="M37" s="56"/>
+      <c r="N37" s="56"/>
+      <c r="O37" s="63"/>
+      <c r="P37" s="47"/>
+      <c r="Q37" s="56"/>
+    </row>
+    <row r="38" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E38" s="56"/>
+      <c r="F38" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="H38" s="44"/>
+      <c r="I38" s="56"/>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="E39" s="56"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="52"/>
+      <c r="I39" s="56"/>
+    </row>
+    <row r="40" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E40" s="56"/>
+      <c r="F40" s="56"/>
+      <c r="G40" s="56"/>
+      <c r="H40" s="56"/>
+      <c r="I40" s="56"/>
+      <c r="J40" s="11"/>
+    </row>
+    <row r="41" spans="2:22" ht="18" x14ac:dyDescent="0.25">
       <c r="B41"/>
+      <c r="E41" s="56"/>
+      <c r="F41" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G41" s="18"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="56"/>
       <c r="V41" s="11"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="E42" s="56"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="56"/>
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B43"/>
+      <c r="E43" s="56"/>
+      <c r="F43" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G43" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H43" s="43"/>
+      <c r="I43" s="56"/>
     </row>
     <row r="44" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B44"/>
+      <c r="E44" s="56"/>
+      <c r="F44" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="G44" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H44" s="37">
+        <v>19</v>
+      </c>
+      <c r="I44" s="56"/>
     </row>
     <row r="45" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B45"/>
+      <c r="E45" s="56"/>
+      <c r="F45" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H45" s="62"/>
+      <c r="I45" s="56"/>
       <c r="J45"/>
       <c r="M45"/>
       <c r="N45"/>
@@ -5733,12 +5873,17 @@
       <c r="Q45"/>
       <c r="R45"/>
     </row>
-    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46"/>
-      <c r="F46"/>
-      <c r="G46"/>
-      <c r="H46"/>
-      <c r="I46"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="G46" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="H46" s="44"/>
+      <c r="I46" s="56"/>
       <c r="J46"/>
       <c r="K46"/>
       <c r="L46"/>
@@ -5749,9 +5894,18 @@
     </row>
     <row r="47" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B47"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="52"/>
+      <c r="H47" s="52"/>
+      <c r="I47" s="47"/>
     </row>
     <row r="48" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48"/>
       <c r="U48"/>
       <c r="V48"/>
     </row>
@@ -5852,10 +6006,6 @@
       <c r="V54"/>
     </row>
     <row r="55" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="F55"/>
-      <c r="G55"/>
-      <c r="H55"/>
-      <c r="I55"/>
       <c r="J55"/>
       <c r="K55"/>
       <c r="L55"/>
@@ -5867,10 +6017,6 @@
       <c r="V55"/>
     </row>
     <row r="56" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="F56"/>
-      <c r="G56"/>
-      <c r="H56"/>
-      <c r="I56"/>
       <c r="J56"/>
       <c r="K56"/>
       <c r="L56"/>
@@ -5882,10 +6028,6 @@
       <c r="V56"/>
     </row>
     <row r="57" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="F57"/>
-      <c r="G57"/>
-      <c r="H57"/>
-      <c r="I57"/>
       <c r="J57"/>
       <c r="K57"/>
       <c r="L57"/>
@@ -5904,10 +6046,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="P4:S24"/>
+  <dimension ref="B4:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5994,53 +6136,54 @@
     </row>
     <row r="16" spans="16:19" ht="15" x14ac:dyDescent="0.25">
       <c r="P16"/>
-      <c r="Q16"/>
+      <c r="Q16" s="46"/>
       <c r="R16"/>
       <c r="S16"/>
     </row>
-    <row r="17" spans="16:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:19" ht="15" x14ac:dyDescent="0.25">
       <c r="P17"/>
       <c r="Q17"/>
       <c r="R17"/>
       <c r="S17"/>
     </row>
-    <row r="18" spans="16:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:19" ht="15" x14ac:dyDescent="0.25">
       <c r="P18"/>
       <c r="Q18"/>
       <c r="R18"/>
       <c r="S18"/>
     </row>
-    <row r="19" spans="16:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" ht="15" x14ac:dyDescent="0.25">
       <c r="P19"/>
       <c r="Q19"/>
       <c r="R19"/>
       <c r="S19"/>
     </row>
-    <row r="20" spans="16:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:19" ht="15" x14ac:dyDescent="0.25">
       <c r="P20"/>
       <c r="Q20"/>
       <c r="R20"/>
       <c r="S20"/>
     </row>
-    <row r="21" spans="16:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" ht="15" x14ac:dyDescent="0.25">
       <c r="P21"/>
       <c r="Q21"/>
       <c r="R21"/>
       <c r="S21"/>
     </row>
-    <row r="22" spans="16:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:19" ht="15" x14ac:dyDescent="0.25">
       <c r="P22"/>
       <c r="Q22"/>
       <c r="R22"/>
       <c r="S22"/>
     </row>
-    <row r="23" spans="16:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:19" ht="15" x14ac:dyDescent="0.25">
+      <c r="B23" s="11"/>
       <c r="P23"/>
       <c r="Q23"/>
       <c r="R23"/>
       <c r="S23"/>
     </row>
-    <row r="24" spans="16:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" ht="15" x14ac:dyDescent="0.25">
       <c r="P24"/>
       <c r="Q24"/>
       <c r="R24"/>

</xml_diff>